<commit_message>
updates to lowcost housing break into parts, problem statement and audience grammarly tidy-up more detail on scenario added audience tags to posts
</commit_message>
<xml_diff>
--- a/resources/england_football_simulation/england_football_exercise_training_log_2017.xlsx
+++ b/resources/england_football_simulation/england_football_exercise_training_log_2017.xlsx
@@ -5294,7 +5294,7 @@
         <v>35734</v>
       </c>
       <c r="D2" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>42795</v>
@@ -5320,7 +5320,7 @@
         <v>35734</v>
       </c>
       <c r="D3" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>42795</v>
@@ -5346,7 +5346,7 @@
         <v>35734</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>42795</v>
@@ -5372,7 +5372,7 @@
         <v>35734</v>
       </c>
       <c r="D5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>42795</v>
@@ -5398,7 +5398,7 @@
         <v>35734</v>
       </c>
       <c r="D6" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>42795</v>
@@ -5424,7 +5424,7 @@
         <v>35734</v>
       </c>
       <c r="D7" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>42795</v>
@@ -5450,7 +5450,7 @@
         <v>35734</v>
       </c>
       <c r="D8" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>42796</v>
@@ -5476,7 +5476,7 @@
         <v>35734</v>
       </c>
       <c r="D9" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>42796</v>
@@ -5502,7 +5502,7 @@
         <v>35734</v>
       </c>
       <c r="D10" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E10" s="1" t="n">
         <v>42796</v>
@@ -5528,7 +5528,7 @@
         <v>35734</v>
       </c>
       <c r="D11" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E11" s="1" t="n">
         <v>42796</v>
@@ -5554,7 +5554,7 @@
         <v>35734</v>
       </c>
       <c r="D12" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>42796</v>
@@ -5580,7 +5580,7 @@
         <v>35734</v>
       </c>
       <c r="D13" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>42796</v>
@@ -5606,7 +5606,7 @@
         <v>35734</v>
       </c>
       <c r="D14" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>42797</v>
@@ -5632,7 +5632,7 @@
         <v>35734</v>
       </c>
       <c r="D15" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>42797</v>
@@ -5658,7 +5658,7 @@
         <v>35734</v>
       </c>
       <c r="D16" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>42797</v>
@@ -5684,7 +5684,7 @@
         <v>35734</v>
       </c>
       <c r="D17" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E17" s="1" t="n">
         <v>42797</v>
@@ -5710,7 +5710,7 @@
         <v>35734</v>
       </c>
       <c r="D18" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>42797</v>
@@ -5736,7 +5736,7 @@
         <v>35734</v>
       </c>
       <c r="D19" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E19" s="1" t="n">
         <v>42797</v>
@@ -5762,7 +5762,7 @@
         <v>35734</v>
       </c>
       <c r="D20" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>42798</v>
@@ -5788,7 +5788,7 @@
         <v>35734</v>
       </c>
       <c r="D21" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E21" s="1" t="n">
         <v>42798</v>
@@ -5814,7 +5814,7 @@
         <v>35734</v>
       </c>
       <c r="D22" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E22" s="1" t="n">
         <v>42798</v>
@@ -5840,7 +5840,7 @@
         <v>35734</v>
       </c>
       <c r="D23" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E23" s="1" t="n">
         <v>42798</v>
@@ -5866,7 +5866,7 @@
         <v>35734</v>
       </c>
       <c r="D24" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E24" s="1" t="n">
         <v>42798</v>
@@ -5892,7 +5892,7 @@
         <v>35734</v>
       </c>
       <c r="D25" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E25" s="1" t="n">
         <v>42798</v>
@@ -5918,7 +5918,7 @@
         <v>35734</v>
       </c>
       <c r="D26" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E26" s="1" t="n">
         <v>42799</v>
@@ -5944,7 +5944,7 @@
         <v>35734</v>
       </c>
       <c r="D27" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E27" s="1" t="n">
         <v>42799</v>
@@ -5970,7 +5970,7 @@
         <v>35734</v>
       </c>
       <c r="D28" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E28" s="1" t="n">
         <v>42799</v>
@@ -5996,7 +5996,7 @@
         <v>35734</v>
       </c>
       <c r="D29" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E29" s="1" t="n">
         <v>42799</v>
@@ -6022,7 +6022,7 @@
         <v>35734</v>
       </c>
       <c r="D30" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E30" s="1" t="n">
         <v>42799</v>
@@ -6048,7 +6048,7 @@
         <v>35734</v>
       </c>
       <c r="D31" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E31" s="1" t="n">
         <v>42799</v>
@@ -6074,7 +6074,7 @@
         <v>35734</v>
       </c>
       <c r="D32" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E32" s="1" t="n">
         <v>42800</v>
@@ -6098,7 +6098,7 @@
         <v>35734</v>
       </c>
       <c r="D33" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E33" s="1" t="n">
         <v>42800</v>
@@ -6122,7 +6122,7 @@
         <v>35734</v>
       </c>
       <c r="D34" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E34" s="1" t="n">
         <v>42800</v>
@@ -6146,7 +6146,7 @@
         <v>35734</v>
       </c>
       <c r="D35" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E35" s="1" t="n">
         <v>42800</v>
@@ -6170,7 +6170,7 @@
         <v>35734</v>
       </c>
       <c r="D36" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E36" s="1" t="n">
         <v>42800</v>
@@ -6194,7 +6194,7 @@
         <v>35734</v>
       </c>
       <c r="D37" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E37" s="1" t="n">
         <v>42800</v>
@@ -6218,7 +6218,7 @@
         <v>35734</v>
       </c>
       <c r="D38" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E38" s="1" t="n">
         <v>42801</v>
@@ -6244,7 +6244,7 @@
         <v>35734</v>
       </c>
       <c r="D39" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E39" s="1" t="n">
         <v>42801</v>
@@ -6270,7 +6270,7 @@
         <v>35734</v>
       </c>
       <c r="D40" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E40" s="1" t="n">
         <v>42801</v>
@@ -6296,7 +6296,7 @@
         <v>35734</v>
       </c>
       <c r="D41" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E41" s="1" t="n">
         <v>42801</v>
@@ -6322,7 +6322,7 @@
         <v>35734</v>
       </c>
       <c r="D42" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E42" s="1" t="n">
         <v>42801</v>
@@ -6348,7 +6348,7 @@
         <v>35734</v>
       </c>
       <c r="D43" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E43" s="1" t="n">
         <v>42801</v>
@@ -6374,7 +6374,7 @@
         <v>35734</v>
       </c>
       <c r="D44" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E44" s="1" t="n">
         <v>42802</v>
@@ -6398,7 +6398,7 @@
         <v>35734</v>
       </c>
       <c r="D45" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E45" s="1" t="n">
         <v>42802</v>
@@ -6422,7 +6422,7 @@
         <v>35734</v>
       </c>
       <c r="D46" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E46" s="1" t="n">
         <v>42802</v>
@@ -6446,7 +6446,7 @@
         <v>35734</v>
       </c>
       <c r="D47" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E47" s="1" t="n">
         <v>42802</v>
@@ -6470,7 +6470,7 @@
         <v>35734</v>
       </c>
       <c r="D48" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E48" s="1" t="n">
         <v>42802</v>
@@ -6494,7 +6494,7 @@
         <v>35734</v>
       </c>
       <c r="D49" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E49" s="1" t="n">
         <v>42802</v>
@@ -6518,7 +6518,7 @@
         <v>35734</v>
       </c>
       <c r="D50" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E50" s="1" t="n">
         <v>42803</v>
@@ -6544,7 +6544,7 @@
         <v>35734</v>
       </c>
       <c r="D51" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E51" s="1" t="n">
         <v>42803</v>
@@ -6570,7 +6570,7 @@
         <v>35734</v>
       </c>
       <c r="D52" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E52" s="1" t="n">
         <v>42803</v>
@@ -6596,7 +6596,7 @@
         <v>35734</v>
       </c>
       <c r="D53" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E53" s="1" t="n">
         <v>42803</v>
@@ -6622,7 +6622,7 @@
         <v>35734</v>
       </c>
       <c r="D54" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E54" s="1" t="n">
         <v>42803</v>
@@ -6648,7 +6648,7 @@
         <v>35734</v>
       </c>
       <c r="D55" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E55" s="1" t="n">
         <v>42803</v>
@@ -6674,7 +6674,7 @@
         <v>35734</v>
       </c>
       <c r="D56" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E56" s="1" t="n">
         <v>42804</v>
@@ -6700,7 +6700,7 @@
         <v>35734</v>
       </c>
       <c r="D57" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E57" s="1" t="n">
         <v>42804</v>
@@ -6726,7 +6726,7 @@
         <v>35734</v>
       </c>
       <c r="D58" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E58" s="1" t="n">
         <v>42804</v>
@@ -6752,7 +6752,7 @@
         <v>35734</v>
       </c>
       <c r="D59" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E59" s="1" t="n">
         <v>42804</v>
@@ -6778,7 +6778,7 @@
         <v>35734</v>
       </c>
       <c r="D60" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E60" s="1" t="n">
         <v>42804</v>
@@ -6804,7 +6804,7 @@
         <v>35734</v>
       </c>
       <c r="D61" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E61" s="1" t="n">
         <v>42804</v>
@@ -6830,7 +6830,7 @@
         <v>35734</v>
       </c>
       <c r="D62" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E62" s="1" t="n">
         <v>42805</v>
@@ -6856,7 +6856,7 @@
         <v>35734</v>
       </c>
       <c r="D63" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E63" s="1" t="n">
         <v>42805</v>
@@ -6882,7 +6882,7 @@
         <v>35734</v>
       </c>
       <c r="D64" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E64" s="1" t="n">
         <v>42805</v>
@@ -6908,7 +6908,7 @@
         <v>35734</v>
       </c>
       <c r="D65" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E65" s="1" t="n">
         <v>42805</v>
@@ -6934,7 +6934,7 @@
         <v>35734</v>
       </c>
       <c r="D66" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E66" s="1" t="n">
         <v>42805</v>
@@ -6960,7 +6960,7 @@
         <v>35734</v>
       </c>
       <c r="D67" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E67" s="1" t="n">
         <v>42805</v>
@@ -6986,7 +6986,7 @@
         <v>35734</v>
       </c>
       <c r="D68" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E68" s="1" t="n">
         <v>42806</v>
@@ -7012,7 +7012,7 @@
         <v>35734</v>
       </c>
       <c r="D69" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E69" s="1" t="n">
         <v>42806</v>
@@ -7038,7 +7038,7 @@
         <v>35734</v>
       </c>
       <c r="D70" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E70" s="1" t="n">
         <v>42806</v>
@@ -7064,7 +7064,7 @@
         <v>35734</v>
       </c>
       <c r="D71" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E71" s="1" t="n">
         <v>42806</v>
@@ -7090,7 +7090,7 @@
         <v>35734</v>
       </c>
       <c r="D72" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E72" s="1" t="n">
         <v>42806</v>
@@ -7116,7 +7116,7 @@
         <v>35734</v>
       </c>
       <c r="D73" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E73" s="1" t="n">
         <v>42806</v>
@@ -7142,7 +7142,7 @@
         <v>35734</v>
       </c>
       <c r="D74" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E74" s="1" t="n">
         <v>42807</v>
@@ -7168,7 +7168,7 @@
         <v>35734</v>
       </c>
       <c r="D75" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E75" s="1" t="n">
         <v>42807</v>
@@ -7194,7 +7194,7 @@
         <v>35734</v>
       </c>
       <c r="D76" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E76" s="1" t="n">
         <v>42807</v>
@@ -7220,7 +7220,7 @@
         <v>35734</v>
       </c>
       <c r="D77" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E77" s="1" t="n">
         <v>42807</v>
@@ -7246,7 +7246,7 @@
         <v>35734</v>
       </c>
       <c r="D78" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E78" s="1" t="n">
         <v>42807</v>
@@ -7272,7 +7272,7 @@
         <v>35734</v>
       </c>
       <c r="D79" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E79" s="1" t="n">
         <v>42807</v>
@@ -7298,7 +7298,7 @@
         <v>35734</v>
       </c>
       <c r="D80" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E80" s="1" t="n">
         <v>42808</v>
@@ -7322,7 +7322,7 @@
         <v>35734</v>
       </c>
       <c r="D81" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E81" s="1" t="n">
         <v>42808</v>
@@ -7346,7 +7346,7 @@
         <v>35734</v>
       </c>
       <c r="D82" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E82" s="1" t="n">
         <v>42808</v>
@@ -7370,7 +7370,7 @@
         <v>35734</v>
       </c>
       <c r="D83" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E83" s="1" t="n">
         <v>42808</v>
@@ -7394,7 +7394,7 @@
         <v>35734</v>
       </c>
       <c r="D84" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E84" s="1" t="n">
         <v>42808</v>
@@ -7418,7 +7418,7 @@
         <v>35734</v>
       </c>
       <c r="D85" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E85" s="1" t="n">
         <v>42808</v>
@@ -7442,7 +7442,7 @@
         <v>35734</v>
       </c>
       <c r="D86" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E86" s="1" t="n">
         <v>42809</v>
@@ -7468,7 +7468,7 @@
         <v>35734</v>
       </c>
       <c r="D87" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E87" s="1" t="n">
         <v>42809</v>
@@ -7494,7 +7494,7 @@
         <v>35734</v>
       </c>
       <c r="D88" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E88" s="1" t="n">
         <v>42809</v>
@@ -7520,7 +7520,7 @@
         <v>35734</v>
       </c>
       <c r="D89" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E89" s="1" t="n">
         <v>42809</v>
@@ -7546,7 +7546,7 @@
         <v>35734</v>
       </c>
       <c r="D90" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E90" s="1" t="n">
         <v>42809</v>
@@ -7572,7 +7572,7 @@
         <v>35734</v>
       </c>
       <c r="D91" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E91" s="1" t="n">
         <v>42809</v>
@@ -7598,7 +7598,7 @@
         <v>35734</v>
       </c>
       <c r="D92" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E92" s="1" t="n">
         <v>42810</v>
@@ -7624,7 +7624,7 @@
         <v>35734</v>
       </c>
       <c r="D93" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E93" s="1" t="n">
         <v>42810</v>
@@ -7650,7 +7650,7 @@
         <v>35734</v>
       </c>
       <c r="D94" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E94" s="1" t="n">
         <v>42810</v>
@@ -7676,7 +7676,7 @@
         <v>35734</v>
       </c>
       <c r="D95" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E95" s="1" t="n">
         <v>42810</v>
@@ -7702,7 +7702,7 @@
         <v>35734</v>
       </c>
       <c r="D96" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E96" s="1" t="n">
         <v>42810</v>
@@ -7728,7 +7728,7 @@
         <v>35734</v>
       </c>
       <c r="D97" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E97" s="1" t="n">
         <v>42810</v>
@@ -7754,7 +7754,7 @@
         <v>35734</v>
       </c>
       <c r="D98" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E98" s="1" t="n">
         <v>42811</v>
@@ -7780,7 +7780,7 @@
         <v>35734</v>
       </c>
       <c r="D99" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E99" s="1" t="n">
         <v>42811</v>
@@ -7806,7 +7806,7 @@
         <v>35734</v>
       </c>
       <c r="D100" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E100" s="1" t="n">
         <v>42811</v>
@@ -7832,7 +7832,7 @@
         <v>35734</v>
       </c>
       <c r="D101" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E101" s="1" t="n">
         <v>42811</v>
@@ -7858,7 +7858,7 @@
         <v>35734</v>
       </c>
       <c r="D102" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E102" s="1" t="n">
         <v>42811</v>
@@ -7884,7 +7884,7 @@
         <v>35734</v>
       </c>
       <c r="D103" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E103" s="1" t="n">
         <v>42811</v>
@@ -7910,7 +7910,7 @@
         <v>35734</v>
       </c>
       <c r="D104" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E104" s="1" t="n">
         <v>42812</v>
@@ -7934,7 +7934,7 @@
         <v>35734</v>
       </c>
       <c r="D105" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E105" s="1" t="n">
         <v>42812</v>
@@ -7958,7 +7958,7 @@
         <v>35734</v>
       </c>
       <c r="D106" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E106" s="1" t="n">
         <v>42812</v>
@@ -7982,7 +7982,7 @@
         <v>35734</v>
       </c>
       <c r="D107" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E107" s="1" t="n">
         <v>42812</v>
@@ -8006,7 +8006,7 @@
         <v>35734</v>
       </c>
       <c r="D108" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E108" s="1" t="n">
         <v>42812</v>
@@ -8030,7 +8030,7 @@
         <v>35734</v>
       </c>
       <c r="D109" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E109" s="1" t="n">
         <v>42812</v>
@@ -8054,7 +8054,7 @@
         <v>35734</v>
       </c>
       <c r="D110" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E110" s="1" t="n">
         <v>42813</v>
@@ -8080,7 +8080,7 @@
         <v>35734</v>
       </c>
       <c r="D111" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E111" s="1" t="n">
         <v>42813</v>
@@ -8106,7 +8106,7 @@
         <v>35734</v>
       </c>
       <c r="D112" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E112" s="1" t="n">
         <v>42813</v>
@@ -8132,7 +8132,7 @@
         <v>35734</v>
       </c>
       <c r="D113" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E113" s="1" t="n">
         <v>42813</v>
@@ -8158,7 +8158,7 @@
         <v>35734</v>
       </c>
       <c r="D114" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E114" s="1" t="n">
         <v>42813</v>
@@ -8184,7 +8184,7 @@
         <v>35734</v>
       </c>
       <c r="D115" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E115" s="1" t="n">
         <v>42813</v>
@@ -8210,7 +8210,7 @@
         <v>35734</v>
       </c>
       <c r="D116" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E116" s="1" t="n">
         <v>42814</v>
@@ -8236,7 +8236,7 @@
         <v>35734</v>
       </c>
       <c r="D117" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E117" s="1" t="n">
         <v>42814</v>
@@ -8262,7 +8262,7 @@
         <v>35734</v>
       </c>
       <c r="D118" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E118" s="1" t="n">
         <v>42814</v>
@@ -8288,7 +8288,7 @@
         <v>35734</v>
       </c>
       <c r="D119" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E119" s="1" t="n">
         <v>42814</v>
@@ -8314,7 +8314,7 @@
         <v>35734</v>
       </c>
       <c r="D120" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E120" s="1" t="n">
         <v>42814</v>
@@ -8340,7 +8340,7 @@
         <v>35734</v>
       </c>
       <c r="D121" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E121" s="1" t="n">
         <v>42814</v>
@@ -8366,7 +8366,7 @@
         <v>35734</v>
       </c>
       <c r="D122" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E122" s="1" t="n">
         <v>42815</v>
@@ -8390,7 +8390,7 @@
         <v>35734</v>
       </c>
       <c r="D123" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E123" s="1" t="n">
         <v>42815</v>
@@ -8414,7 +8414,7 @@
         <v>35734</v>
       </c>
       <c r="D124" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E124" s="1" t="n">
         <v>42815</v>
@@ -8438,7 +8438,7 @@
         <v>35734</v>
       </c>
       <c r="D125" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E125" s="1" t="n">
         <v>42815</v>
@@ -8462,7 +8462,7 @@
         <v>35734</v>
       </c>
       <c r="D126" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E126" s="1" t="n">
         <v>42815</v>
@@ -8486,7 +8486,7 @@
         <v>35734</v>
       </c>
       <c r="D127" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E127" s="1" t="n">
         <v>42815</v>
@@ -8510,7 +8510,7 @@
         <v>35734</v>
       </c>
       <c r="D128" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E128" s="1" t="n">
         <v>42816</v>
@@ -8534,7 +8534,7 @@
         <v>35734</v>
       </c>
       <c r="D129" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E129" s="1" t="n">
         <v>42816</v>
@@ -8558,7 +8558,7 @@
         <v>35734</v>
       </c>
       <c r="D130" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E130" s="1" t="n">
         <v>42816</v>
@@ -8582,7 +8582,7 @@
         <v>35734</v>
       </c>
       <c r="D131" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E131" s="1" t="n">
         <v>42816</v>
@@ -8606,7 +8606,7 @@
         <v>35734</v>
       </c>
       <c r="D132" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E132" s="1" t="n">
         <v>42816</v>
@@ -8630,7 +8630,7 @@
         <v>35734</v>
       </c>
       <c r="D133" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E133" s="1" t="n">
         <v>42816</v>
@@ -8654,7 +8654,7 @@
         <v>35734</v>
       </c>
       <c r="D134" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E134" s="1" t="n">
         <v>42817</v>
@@ -8680,7 +8680,7 @@
         <v>35734</v>
       </c>
       <c r="D135" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E135" s="1" t="n">
         <v>42817</v>
@@ -8706,7 +8706,7 @@
         <v>35734</v>
       </c>
       <c r="D136" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E136" s="1" t="n">
         <v>42817</v>
@@ -8732,7 +8732,7 @@
         <v>35734</v>
       </c>
       <c r="D137" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E137" s="1" t="n">
         <v>42817</v>
@@ -8758,7 +8758,7 @@
         <v>35734</v>
       </c>
       <c r="D138" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E138" s="1" t="n">
         <v>42817</v>
@@ -8784,7 +8784,7 @@
         <v>35734</v>
       </c>
       <c r="D139" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E139" s="1" t="n">
         <v>42817</v>
@@ -8810,7 +8810,7 @@
         <v>35734</v>
       </c>
       <c r="D140" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E140" s="1" t="n">
         <v>42818</v>
@@ -8836,7 +8836,7 @@
         <v>35734</v>
       </c>
       <c r="D141" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E141" s="1" t="n">
         <v>42818</v>
@@ -8862,7 +8862,7 @@
         <v>35734</v>
       </c>
       <c r="D142" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E142" s="1" t="n">
         <v>42818</v>
@@ -8888,7 +8888,7 @@
         <v>35734</v>
       </c>
       <c r="D143" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E143" s="1" t="n">
         <v>42818</v>
@@ -8914,7 +8914,7 @@
         <v>35734</v>
       </c>
       <c r="D144" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E144" s="1" t="n">
         <v>42818</v>
@@ -8940,7 +8940,7 @@
         <v>35734</v>
       </c>
       <c r="D145" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E145" s="1" t="n">
         <v>42818</v>
@@ -8966,7 +8966,7 @@
         <v>35734</v>
       </c>
       <c r="D146" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E146" s="1" t="n">
         <v>42819</v>
@@ -8992,7 +8992,7 @@
         <v>35734</v>
       </c>
       <c r="D147" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E147" s="1" t="n">
         <v>42819</v>
@@ -9018,7 +9018,7 @@
         <v>35734</v>
       </c>
       <c r="D148" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E148" s="1" t="n">
         <v>42819</v>
@@ -9044,7 +9044,7 @@
         <v>35734</v>
       </c>
       <c r="D149" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E149" s="1" t="n">
         <v>42819</v>
@@ -9070,7 +9070,7 @@
         <v>35734</v>
       </c>
       <c r="D150" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E150" s="1" t="n">
         <v>42819</v>
@@ -9096,7 +9096,7 @@
         <v>35734</v>
       </c>
       <c r="D151" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E151" s="1" t="n">
         <v>42819</v>
@@ -9122,7 +9122,7 @@
         <v>35734</v>
       </c>
       <c r="D152" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E152" s="1" t="n">
         <v>42820</v>
@@ -9148,7 +9148,7 @@
         <v>35734</v>
       </c>
       <c r="D153" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E153" s="1" t="n">
         <v>42820</v>
@@ -9174,7 +9174,7 @@
         <v>35734</v>
       </c>
       <c r="D154" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E154" s="1" t="n">
         <v>42820</v>
@@ -9200,7 +9200,7 @@
         <v>35734</v>
       </c>
       <c r="D155" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E155" s="1" t="n">
         <v>42820</v>
@@ -9226,7 +9226,7 @@
         <v>35734</v>
       </c>
       <c r="D156" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E156" s="1" t="n">
         <v>42820</v>
@@ -9252,7 +9252,7 @@
         <v>35734</v>
       </c>
       <c r="D157" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E157" s="1" t="n">
         <v>42820</v>
@@ -9278,7 +9278,7 @@
         <v>35734</v>
       </c>
       <c r="D158" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E158" s="1" t="n">
         <v>42821</v>
@@ -9304,7 +9304,7 @@
         <v>35734</v>
       </c>
       <c r="D159" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E159" s="1" t="n">
         <v>42821</v>
@@ -9330,7 +9330,7 @@
         <v>35734</v>
       </c>
       <c r="D160" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E160" s="1" t="n">
         <v>42821</v>
@@ -9356,7 +9356,7 @@
         <v>35734</v>
       </c>
       <c r="D161" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E161" s="1" t="n">
         <v>42821</v>
@@ -9382,7 +9382,7 @@
         <v>35734</v>
       </c>
       <c r="D162" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E162" s="1" t="n">
         <v>42821</v>
@@ -9408,7 +9408,7 @@
         <v>35734</v>
       </c>
       <c r="D163" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E163" s="1" t="n">
         <v>42821</v>
@@ -9434,7 +9434,7 @@
         <v>35734</v>
       </c>
       <c r="D164" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E164" s="1" t="n">
         <v>42822</v>
@@ -9460,7 +9460,7 @@
         <v>35734</v>
       </c>
       <c r="D165" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E165" s="1" t="n">
         <v>42822</v>
@@ -9486,7 +9486,7 @@
         <v>35734</v>
       </c>
       <c r="D166" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E166" s="1" t="n">
         <v>42822</v>
@@ -9512,7 +9512,7 @@
         <v>35734</v>
       </c>
       <c r="D167" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E167" s="1" t="n">
         <v>42822</v>
@@ -9538,7 +9538,7 @@
         <v>35734</v>
       </c>
       <c r="D168" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E168" s="1" t="n">
         <v>42822</v>
@@ -9564,7 +9564,7 @@
         <v>35734</v>
       </c>
       <c r="D169" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E169" s="1" t="n">
         <v>42822</v>

</xml_diff>